<commit_message>
officegen working but unable to create slides from templates, will need to use another library
</commit_message>
<xml_diff>
--- a/test_deck_builder.xlsx
+++ b/test_deck_builder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charliecheesman/code/Ches-ctrl/Sidedeck/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73F7207D-D7D8-0841-8450-F6E3CF6C61EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CE2137-38C2-CD49-8E19-6B9AB562B83F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{47BDB571-75D8-B645-90CC-14D52B179DE3}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Slide Title</t>
   </si>
   <si>
-    <t>Template Name</t>
-  </si>
-  <si>
     <t>Second Page</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>Template</t>
   </si>
 </sst>
 </file>
@@ -414,12 +414,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -428,12 +428,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -441,7 +441,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -457,26 +457,26 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>